<commit_message>
Add Factorise export search
factor: search the dict generated by the json export is now factorised in a helper function
</commit_message>
<xml_diff>
--- a/export/jp_inventory.xlsx
+++ b/export/jp_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArthurBartoli\Documents\Wrk_dir\mazars\pbi inventory\inventory_script\export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\ArthurBartoli\Documents\Wrk_dir\code\python\Inventory_Script\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E54811C9-1882-4870-9411-C0CC23E5FE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2317B014-C5CB-412F-9BCC-06C3F7FA1C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="5" xr2:uid="{DD5FBE24-2FEE-480D-B91B-6627BECF929E}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="5" xr2:uid="{49E1BED9-538B-4848-A95D-C4F2CAF46536}"/>
   </bookViews>
   <sheets>
     <sheet name="Workspaces" sheetId="1" r:id="rId1"/>
@@ -244,13 +244,13 @@
     <t>Admin monitoring</t>
   </si>
   <si>
+    <t>AdminInsights-6a0f4001-4816-48e9-a868-b7795aafe110</t>
+  </si>
+  <si>
     <t>56c6f8c0-ded6-4444-91e6-4835e4023b53</t>
   </si>
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>AdminInsights-6a0f4001-4816-48e9-a868-b7795aafe110</t>
   </si>
   <si>
     <t>2 reports</t>
@@ -331,70 +331,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C351DF22-546E-4ABF-BD45-5B5D7F9AD610}" name="Tableau1" displayName="Tableau1" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{C351DF22-546E-4ABF-BD45-5B5D7F9AD610}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3534DC92-F756-468B-A807-84DCA00E8FD7}" name="Tableau1" displayName="Tableau1" ref="A1:G3" totalsRowShown="0">
+  <autoFilter ref="A1:G3" xr:uid="{3534DC92-F756-468B-A807-84DCA00E8FD7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2ABECA93-4EB6-44AE-AFFC-BC27640D2B3F}" name="type of workspace"/>
-    <tableColumn id="2" xr3:uid="{C2B4BA99-00D5-44C8-8758-D8425FAB050E}" name="reports"/>
-    <tableColumn id="3" xr3:uid="{46FA604C-8723-4458-90BA-7E0F370D1D88}" name="workspaces"/>
-    <tableColumn id="4" xr3:uid="{259971FB-D7DB-407E-97DD-D8B626FB1558}" name="datasets"/>
-    <tableColumn id="5" xr3:uid="{A71E25A1-863B-410E-B327-659901AF4D34}" name="users"/>
-    <tableColumn id="6" xr3:uid="{67F55292-33A1-42AD-8466-84CCC9709DB1}" name="dataflows"/>
-    <tableColumn id="7" xr3:uid="{91379155-76A4-4FEC-8684-CBFDEB243309}" name="dashboards"/>
+    <tableColumn id="1" xr3:uid="{DB3E6498-4329-4C79-884D-B24F249B2944}" name="type of workspace"/>
+    <tableColumn id="2" xr3:uid="{792C466B-F713-4DA4-A51F-E7F887CF9A3C}" name="reports"/>
+    <tableColumn id="3" xr3:uid="{7F0FAE42-72BC-4DFC-8E64-44C2783C3EAA}" name="workspaces"/>
+    <tableColumn id="4" xr3:uid="{6232571C-D9A5-44B1-9B07-672A3C8FC501}" name="datasets"/>
+    <tableColumn id="5" xr3:uid="{FF7E312F-B32F-4CEB-9A66-D3C947D9A9C2}" name="users"/>
+    <tableColumn id="6" xr3:uid="{4B2B4F92-C71D-4599-8EFD-D73828E81A2C}" name="dataflows"/>
+    <tableColumn id="7" xr3:uid="{533FA3B5-09AA-4018-B06C-C97113C83F46}" name="dashboards"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FDF4646-2FDE-4140-9B44-09C84F87603D}" name="Tableau2" displayName="Tableau2" ref="A1:H10" totalsRowShown="0">
-  <autoFilter ref="A1:H10" xr:uid="{6FDF4646-2FDE-4140-9B44-09C84F87603D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B513424-801F-4235-BFF3-0AC06F03F111}" name="Tableau2" displayName="Tableau2" ref="A1:H10" totalsRowShown="0">
+  <autoFilter ref="A1:H10" xr:uid="{3B513424-801F-4235-BFF3-0AC06F03F111}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E4E112F9-283C-4E49-9618-6BA8CE06B615}" name="DataSourceType"/>
-    <tableColumn id="2" xr3:uid="{A59A11CB-F236-4720-ABF0-C05DD7B2629A}" name="DatasetId"/>
-    <tableColumn id="3" xr3:uid="{720339B8-98DA-4BD2-AEDB-3BD532868E5B}" name="DatasetName"/>
-    <tableColumn id="4" xr3:uid="{62267F18-B7FD-4807-BAB5-C4E2053941D0}" name="ConnectionDetails"/>
-    <tableColumn id="5" xr3:uid="{9B425389-1D4B-4DBA-8C6D-55E279345D29}" name="DataSourceId"/>
-    <tableColumn id="6" xr3:uid="{9B15AFD2-02A4-4C04-88E8-32928CB62CE7}" name="ConnectionString"/>
-    <tableColumn id="7" xr3:uid="{22384D13-1DA7-4C14-8722-DB503FBB37D9}" name="GatewayId"/>
-    <tableColumn id="8" xr3:uid="{1D9D54C8-BA62-4D83-A31B-9EB1DF4B33BB}" name="DataSourceName"/>
+    <tableColumn id="1" xr3:uid="{5E2BD166-A006-4AFE-96F4-D9F13B63404D}" name="DataSourceType"/>
+    <tableColumn id="2" xr3:uid="{05E810A5-7C9C-4441-8DE4-17C02D310C34}" name="DatasetId"/>
+    <tableColumn id="3" xr3:uid="{8F98C269-0496-4149-8B32-5448AD04F147}" name="DatasetName"/>
+    <tableColumn id="4" xr3:uid="{FA49D4C6-E882-4A6C-A445-81F87CF36A95}" name="ConnectionDetails"/>
+    <tableColumn id="5" xr3:uid="{0A861758-1C16-4576-BDF0-2A7332A5F976}" name="DataSourceId"/>
+    <tableColumn id="6" xr3:uid="{E894F78A-0AFF-4E43-B92B-DBE391DDB197}" name="ConnectionString"/>
+    <tableColumn id="7" xr3:uid="{11044BF4-04FF-45B9-9376-65446814A2D4}" name="GatewayId"/>
+    <tableColumn id="8" xr3:uid="{7B966CC5-2FF9-469D-BBFE-5AFF6E96F3C7}" name="DataSourceName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3E7D8F58-C5BD-4FFD-A4DB-17C9EAAD823C}" name="Tableau3" displayName="Tableau3" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{3E7D8F58-C5BD-4FFD-A4DB-17C9EAAD823C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9DB25658-A28D-4A00-BE9D-7FDDEF2BD648}" name="Tableau3" displayName="Tableau3" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{9DB25658-A28D-4A00-BE9D-7FDDEF2BD648}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{080859EC-BB3B-4C11-A0B1-98729B4E333D}" name="UPN"/>
-    <tableColumn id="2" xr3:uid="{AC50A555-EA2C-4655-ADF0-8242BA1A0C5C}" name="# Dashboards"/>
-    <tableColumn id="3" xr3:uid="{C6E3F9F1-F4A1-49EC-BA2B-CBAFA16FECFD}" name="# Reports"/>
-    <tableColumn id="4" xr3:uid="{D1F46A07-BDC3-4BA2-A971-56E15A77F095}" name="# Datasets"/>
-    <tableColumn id="5" xr3:uid="{EBAC9B7E-7AAC-4E1A-B554-725E8B036D3A}" name="Workspace Name"/>
+    <tableColumn id="1" xr3:uid="{36A1DB18-A7D2-468B-880E-BFCDE61A0D85}" name="UPN"/>
+    <tableColumn id="2" xr3:uid="{679A38A6-6670-4A8F-ADB1-88218B1C1978}" name="# Dashboards"/>
+    <tableColumn id="3" xr3:uid="{5E37689C-21F8-4657-A979-0F7D41EAA2BE}" name="# Reports"/>
+    <tableColumn id="4" xr3:uid="{E5C30045-9A01-423F-B4DF-3685A112E1AD}" name="# Datasets"/>
+    <tableColumn id="5" xr3:uid="{589B5713-021A-439A-BF2B-D881BE817050}" name="Workspace Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4C2053DD-9D00-417D-9822-F1AE35E1ABD0}" name="Tableau4" displayName="Tableau4" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{4C2053DD-9D00-417D-9822-F1AE35E1ABD0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{688D0C03-3276-43E3-8E0F-FEBF5344A0B3}" name="Tableau4" displayName="Tableau4" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{688D0C03-3276-43E3-8E0F-FEBF5344A0B3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{19091859-5655-410F-986C-C2AC4E531783}" name="DatasetId"/>
-    <tableColumn id="2" xr3:uid="{644E83AF-123B-4DE8-8215-9472769B695E}" name="DatasetName"/>
-    <tableColumn id="3" xr3:uid="{7CD0C8BB-B0F0-49CB-8C24-A37BDBC41460}" name="Gateway Required"/>
+    <tableColumn id="1" xr3:uid="{D12B1EAE-B011-40C5-AD1B-FB1ED0E19574}" name="DatasetId"/>
+    <tableColumn id="2" xr3:uid="{191E9FB7-CDF2-4007-B3B6-8A6E275E48BC}" name="DatasetName"/>
+    <tableColumn id="3" xr3:uid="{EA9E200B-F6C7-4404-A309-9376CCCB875A}" name="Gateway Required"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC90C813-2238-4B5D-88A2-B61B6FB1A1CB}" name="Tableau5" displayName="Tableau5" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{DC90C813-2238-4B5D-88A2-B61B6FB1A1CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3310C3E8-F0E4-4529-8D69-3A6AB0292530}" name="Tableau5" displayName="Tableau5" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{3310C3E8-F0E4-4529-8D69-3A6AB0292530}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{81D8146A-0A14-411C-80DD-556F539997D1}" name="ReportId"/>
-    <tableColumn id="2" xr3:uid="{313FBD9D-926B-4C67-AAA2-4109F7B22FC2}" name="ReportName"/>
+    <tableColumn id="1" xr3:uid="{31599FDD-FF2D-4E7E-A417-5F1D6650D770}" name="ReportId"/>
+    <tableColumn id="2" xr3:uid="{950956D6-FC59-4C2E-BD4C-DE5B84E13A13}" name="ReportName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,7 +696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37037704-50F5-4994-874C-D452E16D87E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6BA3E6-1726-473A-8D25-86636FA9F759}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417ABC51-05CA-4DE9-9FE3-72DE8CCBDCE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A85A6E-1491-4F35-84D0-B665B2D2FFFA}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1299043-F986-4962-98B2-40306E7CFA2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5799A72A-64F1-4FF8-ABED-0BA612DEF0B6}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1139,7 +1139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769F1A3B-D1D4-4890-A151-41A6E8E179B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F4C28A-326D-490D-BB01-A134E29945A1}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1233,6 +1233,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
       <c r="B14" t="s">
         <v>67</v>
       </c>
@@ -1240,21 +1243,18 @@
         <v>60</v>
       </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1278,7 +1278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1E48B5-765D-45C3-8320-57702332C61F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5696A5A-5EF4-4FCC-90F6-C4DB42626205}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1342,7 +1342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC88FA8-3031-4329-95B1-AB33345B41FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E71D2DB-AF85-4323-A439-CB04DF438205}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>